<commit_message>
Used a standard pivot table
</commit_message>
<xml_diff>
--- a/CH-091 Extract from table.xlsx
+++ b/CH-091 Extract from table.xlsx
@@ -8,20 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEF7DC9-664F-450E-9848-BCEE0AAC7E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F2F0FA-AA5E-4334-9A65-8EE5F4CC6FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
     <sheet name="Alt2" sheetId="6" r:id="rId4"/>
+    <sheet name="PivotApproach" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="13" r:id="rId6"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +39,7 @@
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="/I7b3y6w9dWI5DEUXeppQV2jUuCxrv3A0fktCS/dr1s="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="/I7b3y6w9dWI5DEUXeppQV2jUuCxrv3A0fktCS/dr1s="/>
     </ext>
   </extLst>
 </workbook>
@@ -64,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="30">
   <si>
     <t>Question Table: Info</t>
   </si>
@@ -133,6 +137,27 @@
   </si>
   <si>
     <t>Uses Pivotby</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>Dept</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Count of Branch</t>
   </si>
 </sst>
 </file>
@@ -220,7 +245,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,12 +256,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF58508D"/>
         <bgColor rgb="FF58508D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -465,9 +484,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -529,6 +548,8 @@
     </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Intro_Hd" xfId="2" xr:uid="{DFD9014A-B813-42DF-BC0C-06DFCF29FB9F}"/>
@@ -957,6 +978,213 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="mbieg" refreshedDate="45505.910474305558" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="12" xr:uid="{385A04B4-01D3-40C4-B38F-DD2D20F50E36}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B15:D27" sheet="PivotApproach"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Branch" numFmtId="0">
+      <sharedItems count="4">
+        <s v="1"/>
+        <s v="2"/>
+        <s v="3"/>
+        <s v="4"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Dept" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Sales"/>
+        <s v="HR"/>
+        <s v="Finance"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Name" numFmtId="0">
+      <sharedItems count="7">
+        <s v="David"/>
+        <s v="Rose"/>
+        <s v="Omid"/>
+        <s v="Sara"/>
+        <s v="Mike"/>
+        <s v="Stephen"/>
+        <s v="Daniel" u="1"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="12">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{655F10CD-CF8F-48FE-8932-F26A00D2FD8F}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="F15:K23" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
+  <pivotFields count="3">
+    <pivotField axis="axisCol" dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="7">
+        <item x="3"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item m="1" x="6"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="4"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Branch" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1155,7 +1383,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="224" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -2679,8 +2907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F85869F-77CD-4059-AA26-0862A2609328}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4666,8 +4894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3E0D9B-0847-42B9-9F5A-45D930298918}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30:K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5149,8 +5377,32 @@
       <c r="G16" t="str">
         <v>Branch 4</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" t="str" cm="1">
+        <f t="array" ref="I16:I27">_xlfn.LET(
+    _xlpm.n, C3:E6,
+    _xlpm.L, _xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(_xlpm.n &gt; 0, _xlpm.x))),
+    _xlpm.d, _xlpm.L(C2:E2),
+_xlpm.d
+)</f>
+        <v>Sales</v>
+      </c>
+      <c r="K16" t="str" cm="1">
+        <f t="array" ref="K16:M19">_xlfn.LET(
+    _xlpm.n, C3:E6,
+    _xlpm.L, _xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(_xlpm.n &gt; 0, _xlpm.x))),
+    _xlpm.d, _xlpm.L(C2:E2),
+IF(_xlpm.n &gt; 0, C2:E2)
+)</f>
+        <v>Sales</v>
+      </c>
+      <c r="L16" t="str">
+        <v>HR</v>
+      </c>
+      <c r="M16" t="str">
+        <v>Finance</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" t="str">
         <v>David</v>
@@ -5170,8 +5422,20 @@
       <c r="G17" t="str">
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" t="str">
+        <v>HR</v>
+      </c>
+      <c r="K17" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="L17" t="str">
+        <v>HR</v>
+      </c>
+      <c r="M17" t="str">
+        <v>Finance</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" t="str">
         <v>Sara</v>
@@ -5191,8 +5455,20 @@
       <c r="G18" t="str">
         <v>✔</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="K18" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="L18" t="str">
+        <v>HR</v>
+      </c>
+      <c r="M18" t="str">
+        <v>Finance</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" t="str">
         <v>Daniel</v>
@@ -5212,8 +5488,20 @@
       <c r="G19" t="str">
         <v>✔</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I19" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="K19" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="L19" t="str">
+        <v>HR</v>
+      </c>
+      <c r="M19" t="str">
+        <v>Finance</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" t="str">
         <v>Rose</v>
@@ -5233,8 +5521,11 @@
       <c r="G20" t="str">
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" t="str">
+        <v>HR</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" t="str">
         <v>Stephen</v>
@@ -5254,8 +5545,11 @@
       <c r="G21" t="str">
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" t="str">
+        <v>Finance</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" t="str">
         <v>Mike</v>
@@ -5275,8 +5569,11 @@
       <c r="G22" t="str">
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22" t="str">
+        <v>Sales</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="16" t="str">
         <v>Omid</v>
@@ -5296,13 +5593,1831 @@
       <c r="G23" t="str">
         <v>✔</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" t="str">
+        <v>HR</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
+      <c r="I24" t="str">
+        <v>Finance</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="I25" t="str">
+        <v>Sales</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="I26" t="str">
+        <v>HR</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="I27" t="str">
+        <v>Finance</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
+    </row>
+    <row r="29" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+    </row>
+    <row r="30" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="I30" cm="1">
+        <f t="array" ref="I30:K41">_xlfn.LET(
+    _xlpm.n, C3:E6,
+    _xlpm.L, _xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(_xlpm.n &gt; 0, _xlpm.x))),
+    _xlpm.d, _xlpm.L(C2:E2),
+            _xlfn.HSTACK(_xlfn.XMATCH(_xlpm.d, C2:E2), _xlpm.L(_xlpm.n), _xlpm.d)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="J30" t="str">
+        <v>David</v>
+      </c>
+      <c r="K30" t="str">
+        <v>Sales</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="D31" t="str" cm="1">
+        <f t="array" ref="D31:F34">B3:B6&amp;C2:E2</f>
+        <v>1Sales</v>
+      </c>
+      <c r="E31" t="str">
+        <v>1HR</v>
+      </c>
+      <c r="F31" t="str">
+        <v>1Finance</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31" t="str">
+        <v>Rose</v>
+      </c>
+      <c r="K31" t="str">
+        <v>HR</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" t="str">
+        <v>2Sales</v>
+      </c>
+      <c r="E32" t="str">
+        <v>2HR</v>
+      </c>
+      <c r="F32" t="str">
+        <v>2Finance</v>
+      </c>
+      <c r="I32">
+        <v>3</v>
+      </c>
+      <c r="J32" t="str">
+        <v>Omid</v>
+      </c>
+      <c r="K32" t="str">
+        <v>Finance</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+      <c r="D33" t="str">
+        <v>3Sales</v>
+      </c>
+      <c r="E33" t="str">
+        <v>3HR</v>
+      </c>
+      <c r="F33" t="str">
+        <v>3Finance</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33" t="str">
+        <v>Sara</v>
+      </c>
+      <c r="K33" t="str">
+        <v>Sales</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D34" t="str">
+        <v>4Sales</v>
+      </c>
+      <c r="E34" t="str">
+        <v>4HR</v>
+      </c>
+      <c r="F34" t="str">
+        <v>4Finance</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+      <c r="J34" t="str">
+        <v>Rose</v>
+      </c>
+      <c r="K34" t="str">
+        <v>HR</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="I35">
+        <v>3</v>
+      </c>
+      <c r="J35" t="str">
+        <v>Mike</v>
+      </c>
+      <c r="K35" t="str">
+        <v>Finance</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36" t="str">
+        <v>Sara</v>
+      </c>
+      <c r="K36" t="str">
+        <v>Sales</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37" t="str">
+        <v>Stephen</v>
+      </c>
+      <c r="K37" t="str">
+        <v>HR</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+      <c r="I38">
+        <v>3</v>
+      </c>
+      <c r="J38" t="str">
+        <v>Mike</v>
+      </c>
+      <c r="K38" t="str">
+        <v>Finance</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39" t="str">
+        <v>Sara</v>
+      </c>
+      <c r="K39" t="str">
+        <v>Sales</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>2</v>
+      </c>
+      <c r="J40" t="str">
+        <v>Daniel</v>
+      </c>
+      <c r="K40" t="str">
+        <v>HR</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>3</v>
+      </c>
+      <c r="J41" t="str">
+        <v>Omid</v>
+      </c>
+      <c r="K41" t="str">
+        <v>Finance</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87663A00-0F87-4B43-9144-B85EE29B6E21}">
+  <dimension ref="A1:Z1000"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="4" width="12.3984375" customWidth="1"/>
+    <col min="5" max="5" width="12.09765625" customWidth="1"/>
+    <col min="6" max="6" width="13.8984375" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="11.3984375" customWidth="1"/>
+    <col min="9" max="12" width="8" customWidth="1"/>
+    <col min="13" max="26" width="8.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+    </row>
+    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+    </row>
+    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="13">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+    </row>
+    <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="13">
+        <v>3</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+    </row>
+    <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="13">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+    </row>
+    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+    </row>
+    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+    </row>
+    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="12"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+    </row>
+    <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+    </row>
+    <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+    </row>
+    <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="S12" s="6"/>
+    </row>
+    <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" t="str" cm="1">
+        <f t="array" ref="B13:G20">_xlfn.LET(
+    _xlpm.d, C3:E6,
+    _xlpm.f, _xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF({1}, _xlpm.x, _xlpm.d), , 1)),
+    _xlpm.a, _xlpm.f(_xlpm.d),
+    _xlpm.n, _xlpm.f(B3:B6),
+    _xlfn.DROP(
+        _xlfn.PIVOTBY(
+            _xlfn.HSTACK(_xlfn.XMATCH(_xlpm.a, _xlpm.a), _xlpm.a, _xlpm.f(C2:E2)),
+            "Branch " &amp; _xlpm.n,
+            _xlpm.n,
+            _xlfn.LAMBDA(_xlpm.x, REPT("✔", _xlfn.SINGLE(_xlpm.x) &gt; 0)),
+            ,
+            0,
+            ,
+            0
+        ),
+        ,
+        1
+    )
+)</f>
+        <v/>
+      </c>
+      <c r="C13" t="str">
+        <v/>
+      </c>
+      <c r="D13" t="str">
+        <v>Branch 1</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Branch 2</v>
+      </c>
+      <c r="F13" s="6" t="str">
+        <v>Branch 3</v>
+      </c>
+      <c r="G13" s="6" t="str">
+        <v>Branch 4</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="S13" s="6"/>
+    </row>
+    <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" t="str">
+        <v>David</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="D14" t="str">
+        <v>✔</v>
+      </c>
+      <c r="E14" t="str">
+        <v/>
+      </c>
+      <c r="F14" t="str">
+        <v/>
+      </c>
+      <c r="G14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" t="str">
+        <v>Sara</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="D15" t="str">
+        <v/>
+      </c>
+      <c r="E15" t="str">
+        <v>✔</v>
+      </c>
+      <c r="F15" t="str">
+        <v>✔</v>
+      </c>
+      <c r="G15" t="str">
+        <v>✔</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" t="str">
+        <v>Rose</v>
+      </c>
+      <c r="C16" t="str">
+        <v>HR</v>
+      </c>
+      <c r="D16" t="str">
+        <v>✔</v>
+      </c>
+      <c r="E16" t="str">
+        <v>✔</v>
+      </c>
+      <c r="F16" t="str">
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" t="str">
+        <v>Stephen</v>
+      </c>
+      <c r="C17" t="str">
+        <v>HR</v>
+      </c>
+      <c r="D17" t="str">
+        <v/>
+      </c>
+      <c r="E17" t="str">
+        <v/>
+      </c>
+      <c r="F17" t="str">
+        <v>✔</v>
+      </c>
+      <c r="G17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" t="str">
+        <v>Daniel</v>
+      </c>
+      <c r="C18" t="str">
+        <v>HR</v>
+      </c>
+      <c r="D18" t="str">
+        <v/>
+      </c>
+      <c r="E18" t="str">
+        <v/>
+      </c>
+      <c r="F18" t="str">
+        <v/>
+      </c>
+      <c r="G18" t="str">
+        <v>✔</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" t="str">
+        <v>Omid</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="D19" t="str">
+        <v>✔</v>
+      </c>
+      <c r="E19" t="str">
+        <v/>
+      </c>
+      <c r="F19" t="str">
+        <v/>
+      </c>
+      <c r="G19" t="str">
+        <v>✔</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" t="str">
+        <v>Mike</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="D20" t="str">
+        <v/>
+      </c>
+      <c r="E20" t="str">
+        <v>✔</v>
+      </c>
+      <c r="F20" t="str">
+        <v>✔</v>
+      </c>
+      <c r="G20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+    </row>
+    <row r="22" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+    </row>
+    <row r="23" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+    </row>
+    <row r="24" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
@@ -6318,12 +8433,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87663A00-0F87-4B43-9144-B85EE29B6E21}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18DBDBB5-2E9A-41A4-9F03-81DE029D39FA}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6562,7 +8677,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>14</v>
@@ -6747,44 +8862,8 @@
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
-      <c r="B13" t="str" cm="1">
-        <f t="array" ref="B13:G20">_xlfn.LET(
-    _xlpm.d, C3:E6,
-    _xlpm.f, _xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF({1}, _xlpm.x, _xlpm.d), , 1)),
-    _xlpm.a, _xlpm.f(_xlpm.d),
-    _xlpm.n, _xlpm.f(B3:B6),
-    _xlfn.DROP(
-        _xlfn.PIVOTBY(
-            _xlfn.HSTACK(_xlfn.XMATCH(_xlpm.a, _xlpm.a), _xlpm.a, _xlpm.f(C2:E2)),
-            "Branch " &amp; _xlpm.n,
-            _xlpm.n,
-            _xlfn.LAMBDA(_xlpm.x, REPT("✔", _xlfn.SINGLE(_xlpm.x) &gt; 0)),
-            ,
-            0,
-            ,
-            0
-        ),
-        ,
-        1
-    )
-)</f>
-        <v/>
-      </c>
-      <c r="C13" t="str">
-        <v/>
-      </c>
-      <c r="D13" t="str">
-        <v>Branch 1</v>
-      </c>
-      <c r="E13" t="str">
-        <v>Branch 2</v>
-      </c>
-      <c r="F13" s="6" t="str">
-        <v>Branch 3</v>
-      </c>
-      <c r="G13" s="6" t="str">
-        <v>Branch 4</v>
-      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
@@ -6794,189 +8873,407 @@
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="B14" t="str">
-        <v>David</v>
-      </c>
-      <c r="C14" t="str">
-        <v>Sales</v>
-      </c>
-      <c r="D14" t="str">
-        <v>✔</v>
-      </c>
-      <c r="E14" t="str">
-        <v/>
-      </c>
-      <c r="F14" t="str">
-        <v/>
-      </c>
-      <c r="G14" t="str">
-        <v/>
-      </c>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
-      <c r="B15" t="str">
-        <v>Sara</v>
-      </c>
-      <c r="C15" t="str">
-        <v>Sales</v>
-      </c>
-      <c r="D15" t="str">
-        <v/>
-      </c>
-      <c r="E15" t="str">
-        <v>✔</v>
-      </c>
-      <c r="F15" t="str">
-        <v>✔</v>
-      </c>
-      <c r="G15" t="str">
-        <v>✔</v>
+      <c r="B15" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15" t="s">
+        <v>12</v>
+      </c>
+      <c r="P15" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
-      <c r="B16" t="str">
-        <v>Rose</v>
+      <c r="B16" t="str" cm="1">
+        <f t="array" ref="B16:D27">_xlfn.HSTACK(MID(_xlfn.TOCOL(B3:B6&amp;C2:E2),{1,2},{1,10}),_xlfn.TOCOL(C3:E6))</f>
+        <v>1</v>
       </c>
       <c r="C16" t="str">
-        <v>HR</v>
+        <v>Sales</v>
       </c>
       <c r="D16" t="str">
-        <v>✔</v>
-      </c>
-      <c r="E16" t="str">
-        <v>✔</v>
-      </c>
-      <c r="F16" t="str">
-        <v/>
-      </c>
-      <c r="G16" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>David</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16" t="s">
+        <v>13</v>
+      </c>
+      <c r="P16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" t="str">
-        <v>Stephen</v>
+        <v>1</v>
       </c>
       <c r="C17" t="str">
         <v>HR</v>
       </c>
       <c r="D17" t="str">
-        <v/>
-      </c>
-      <c r="E17" t="str">
-        <v/>
-      </c>
-      <c r="F17" t="str">
-        <v>✔</v>
-      </c>
-      <c r="G17" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>Rose</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28">
+        <v>1</v>
+      </c>
+      <c r="J17" s="28">
+        <v>1</v>
+      </c>
+      <c r="K17" s="28">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>3</v>
+      </c>
+      <c r="O17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" t="str">
-        <v>Daniel</v>
+        <v>1</v>
       </c>
       <c r="C18" t="str">
-        <v>HR</v>
+        <v>Finance</v>
       </c>
       <c r="D18" t="str">
-        <v/>
-      </c>
-      <c r="E18" t="str">
-        <v/>
-      </c>
-      <c r="F18" t="str">
-        <v/>
-      </c>
-      <c r="G18" t="str">
-        <v>✔</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>Omid</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="28">
+        <v>1</v>
+      </c>
+      <c r="I18" s="28">
+        <v>1</v>
+      </c>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18" t="s">
+        <v>16</v>
+      </c>
+      <c r="P18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" t="str">
-        <v>Omid</v>
+        <v>2</v>
       </c>
       <c r="C19" t="str">
-        <v>Finance</v>
+        <v>Sales</v>
       </c>
       <c r="D19" t="str">
-        <v>✔</v>
-      </c>
-      <c r="E19" t="str">
-        <v/>
-      </c>
-      <c r="F19" t="str">
-        <v/>
-      </c>
-      <c r="G19" t="str">
-        <v>✔</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>Sara</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28">
+        <v>1</v>
+      </c>
+      <c r="K19" s="28"/>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="O19" t="s">
+        <v>13</v>
+      </c>
+      <c r="P19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" t="str">
+        <v>2</v>
+      </c>
+      <c r="C20" t="str">
+        <v>HR</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Rose</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
+      <c r="O20" t="s">
+        <v>17</v>
+      </c>
+      <c r="P20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" t="str">
+        <v>2</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="D21" t="str">
         <v>Mike</v>
       </c>
-      <c r="C20" t="str">
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="28">
+        <v>1</v>
+      </c>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21" t="s">
+        <v>16</v>
+      </c>
+      <c r="P21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" t="str">
+        <v>3</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Sara</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="28">
+        <v>1</v>
+      </c>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="O22" t="s">
+        <v>18</v>
+      </c>
+      <c r="P22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16" t="str">
+        <v>3</v>
+      </c>
+      <c r="C23" s="16" t="str">
+        <v>HR</v>
+      </c>
+      <c r="D23" s="16" t="str">
+        <v>Stephen</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28">
+        <v>1</v>
+      </c>
+      <c r="J23" s="28">
+        <v>1</v>
+      </c>
+      <c r="K23" s="28"/>
+      <c r="N23">
+        <v>3</v>
+      </c>
+      <c r="O23" t="s">
+        <v>17</v>
+      </c>
+      <c r="P23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16" t="str">
+        <v>3</v>
+      </c>
+      <c r="C24" s="16" t="str">
         <v>Finance</v>
       </c>
-      <c r="D20" t="str">
-        <v/>
-      </c>
-      <c r="E20" t="str">
-        <v>✔</v>
-      </c>
-      <c r="F20" t="str">
-        <v>✔</v>
-      </c>
-      <c r="G20" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-    </row>
-    <row r="22" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-    </row>
-    <row r="23" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-    </row>
-    <row r="24" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-    </row>
-    <row r="25" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="16" t="str">
+        <v>Mike</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24" t="s">
+        <v>16</v>
+      </c>
+      <c r="P24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
-    </row>
-    <row r="26" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" t="str">
+        <v>4</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Sara</v>
+      </c>
+      <c r="N25">
+        <v>2</v>
+      </c>
+      <c r="O25" t="s">
+        <v>19</v>
+      </c>
+      <c r="P25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
+      <c r="B26" s="16" t="str">
+        <v>4</v>
+      </c>
+      <c r="C26" s="16" t="str">
+        <v>HR</v>
+      </c>
+      <c r="D26" s="16" t="str">
+        <v>David</v>
+      </c>
       <c r="E26" s="16"/>
-    </row>
-    <row r="27" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N26">
+        <v>3</v>
+      </c>
+      <c r="O26" t="s">
+        <v>14</v>
+      </c>
+      <c r="P26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
-    </row>
-    <row r="28" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" t="str">
+        <v>4</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Omid</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
     </row>
-    <row r="29" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
     </row>
-    <row r="30" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
     </row>
-    <row r="31" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
     </row>
-    <row r="32" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
     </row>

</xml_diff>

<commit_message>
Used custom format to deal with final form
</commit_message>
<xml_diff>
--- a/CH-091 Extract from table.xlsx
+++ b/CH-091 Extract from table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F2F0FA-AA5E-4334-9A65-8EE5F4CC6FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0454BE75-D0A7-47FB-BFB4-27A268D183D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId6"/>
+    <pivotCache cacheId="14" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -164,6 +164,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="&quot;Branch &quot;@"/>
+    <numFmt numFmtId="167" formatCode="[=0]&quot;&quot;;[=1]\✔;"/>
+  </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -486,7 +490,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -530,6 +534,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -540,16 +553,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Intro_Hd" xfId="2" xr:uid="{DFD9014A-B813-42DF-BC0C-06DFCF29FB9F}"/>
@@ -1085,7 +1094,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{655F10CD-CF8F-48FE-8932-F26A00D2FD8F}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{655F10CD-CF8F-48FE-8932-F26A00D2FD8F}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="F15:K23" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -1399,6 +1408,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1431,21 +1443,21 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="22"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="27"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1" t="s">
@@ -2907,8 +2919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F85869F-77CD-4059-AA26-0862A2609328}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13:K19"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2927,23 +2939,23 @@
   <sheetData>
     <row r="1" spans="1:28" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="22"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="27"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -3039,7 +3051,7 @@
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
       <c r="O3" s="6"/>
-      <c r="P3" s="25" t="str">
+      <c r="P3" s="19" t="str">
         <f>I3&amp;J3</f>
         <v>DavidSales</v>
       </c>
@@ -3090,7 +3102,7 @@
         <v>15</v>
       </c>
       <c r="O4" s="6"/>
-      <c r="P4" s="25" t="str">
+      <c r="P4" s="19" t="str">
         <f t="shared" ref="P4:P9" si="0">I4&amp;J4</f>
         <v>SaraSales</v>
       </c>
@@ -3139,7 +3151,7 @@
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
       <c r="O5" s="6"/>
-      <c r="P5" s="25" t="str">
+      <c r="P5" s="19" t="str">
         <f t="shared" si="0"/>
         <v>RoseHR</v>
       </c>
@@ -3186,7 +3198,7 @@
       </c>
       <c r="N6" s="12"/>
       <c r="O6" s="6"/>
-      <c r="P6" s="25" t="str">
+      <c r="P6" s="19" t="str">
         <f t="shared" si="0"/>
         <v>StephenHR</v>
       </c>
@@ -3221,7 +3233,7 @@
         <v>15</v>
       </c>
       <c r="O7" s="6"/>
-      <c r="P7" s="25" t="str">
+      <c r="P7" s="19" t="str">
         <f t="shared" si="0"/>
         <v>DavidHR</v>
       </c>
@@ -3258,7 +3270,7 @@
         <v>15</v>
       </c>
       <c r="O8" s="6"/>
-      <c r="P8" s="25" t="str">
+      <c r="P8" s="19" t="str">
         <f t="shared" si="0"/>
         <v>OmidFinance</v>
       </c>
@@ -3295,7 +3307,7 @@
       </c>
       <c r="N9" s="12"/>
       <c r="O9" s="6"/>
-      <c r="P9" s="25" t="str">
+      <c r="P9" s="19" t="str">
         <f t="shared" si="0"/>
         <v>MikeFinance</v>
       </c>
@@ -3380,16 +3392,16 @@
         <f t="array" ref="B13:B24">_xlfn.TOCOL(B3:B6&amp;C2:E2)</f>
         <v>1Sales</v>
       </c>
-      <c r="D13" s="23" t="str" cm="1">
+      <c r="D13" s="17" t="str" cm="1">
         <f t="array" ref="D13:D24">TRIM(_xlfn.TOCOL(C3:E6))</f>
         <v>David</v>
       </c>
       <c r="E13" t="str">
-        <f>RIGHT(B13,LEN(B13)-1)</f>
+        <f t="shared" ref="E13:E24" si="1">RIGHT(B13,LEN(B13)-1)</f>
         <v>Sales</v>
       </c>
       <c r="F13" t="str">
-        <f>"Branch "&amp;LEFT(B13,1)</f>
+        <f t="shared" ref="F13:F24" si="2">"Branch "&amp;LEFT(B13,1)</f>
         <v>Branch 1</v>
       </c>
       <c r="G13" t="str">
@@ -3418,19 +3430,19 @@
       <c r="B14" t="str">
         <v>1HR</v>
       </c>
-      <c r="D14" s="23" t="str">
+      <c r="D14" s="17" t="str">
         <v>Rose</v>
       </c>
       <c r="E14" t="str">
-        <f>RIGHT(B14,LEN(B14)-1)</f>
+        <f t="shared" si="1"/>
         <v>HR</v>
       </c>
       <c r="F14" t="str">
-        <f>"Branch "&amp;LEFT(B14,1)</f>
+        <f t="shared" si="2"/>
         <v>Branch 1</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" ref="G14:G24" si="1">_xlfn.CONCAT(D14:F14)</f>
+        <f t="shared" ref="G14:G24" si="3">_xlfn.CONCAT(D14:F14)</f>
         <v>RoseHRBranch 1</v>
       </c>
       <c r="I14" t="str">
@@ -3440,7 +3452,7 @@
         <v>HR</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" ref="K14:K19" si="2">I14&amp;J14</f>
+        <f t="shared" ref="K14:K19" si="4">I14&amp;J14</f>
         <v>RoseHR</v>
       </c>
       <c r="N14">
@@ -3452,19 +3464,19 @@
       <c r="B15" t="str">
         <v>1Finance</v>
       </c>
-      <c r="D15" s="23" t="str">
+      <c r="D15" s="17" t="str">
         <v>Omid</v>
       </c>
       <c r="E15" t="str">
-        <f>RIGHT(B15,LEN(B15)-1)</f>
+        <f t="shared" si="1"/>
         <v>Finance</v>
       </c>
       <c r="F15" t="str">
-        <f>"Branch "&amp;LEFT(B15,1)</f>
+        <f t="shared" si="2"/>
         <v>Branch 1</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OmidFinanceBranch 1</v>
       </c>
       <c r="I15" t="str">
@@ -3474,7 +3486,7 @@
         <v>Finance</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>OmidFinance</v>
       </c>
       <c r="N15">
@@ -3486,19 +3498,19 @@
       <c r="B16" t="str">
         <v>2Sales</v>
       </c>
-      <c r="D16" s="23" t="str">
+      <c r="D16" s="17" t="str">
         <v>Sara</v>
       </c>
       <c r="E16" t="str">
-        <f>RIGHT(B16,LEN(B16)-1)</f>
+        <f t="shared" si="1"/>
         <v>Sales</v>
       </c>
       <c r="F16" t="str">
-        <f>"Branch "&amp;LEFT(B16,1)</f>
+        <f t="shared" si="2"/>
         <v>Branch 2</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>SaraSalesBranch 2</v>
       </c>
       <c r="I16" t="str">
@@ -3508,7 +3520,7 @@
         <v>Sales</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>SaraSales</v>
       </c>
       <c r="N16">
@@ -3520,19 +3532,19 @@
       <c r="B17" t="str">
         <v>2HR</v>
       </c>
-      <c r="D17" s="23" t="str">
+      <c r="D17" s="17" t="str">
         <v>Rose</v>
       </c>
       <c r="E17" t="str">
-        <f>RIGHT(B17,LEN(B17)-1)</f>
+        <f t="shared" si="1"/>
         <v>HR</v>
       </c>
       <c r="F17" t="str">
-        <f>"Branch "&amp;LEFT(B17,1)</f>
+        <f t="shared" si="2"/>
         <v>Branch 2</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>RoseHRBranch 2</v>
       </c>
       <c r="I17" t="str">
@@ -3542,7 +3554,7 @@
         <v>Finance</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>MikeFinance</v>
       </c>
       <c r="N17">
@@ -3554,19 +3566,19 @@
       <c r="B18" t="str">
         <v>2Finance</v>
       </c>
-      <c r="D18" s="23" t="str">
+      <c r="D18" s="17" t="str">
         <v>Mike</v>
       </c>
       <c r="E18" t="str">
-        <f>RIGHT(B18,LEN(B18)-1)</f>
+        <f t="shared" si="1"/>
         <v>Finance</v>
       </c>
       <c r="F18" t="str">
-        <f>"Branch "&amp;LEFT(B18,1)</f>
+        <f t="shared" si="2"/>
         <v>Branch 2</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>MikeFinanceBranch 2</v>
       </c>
       <c r="I18" t="str">
@@ -3576,7 +3588,7 @@
         <v>HR</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>StephenHR</v>
       </c>
       <c r="N18">
@@ -3588,19 +3600,19 @@
       <c r="B19" t="str">
         <v>3Sales</v>
       </c>
-      <c r="D19" s="23" t="str">
+      <c r="D19" s="17" t="str">
         <v>Sara</v>
       </c>
       <c r="E19" t="str">
-        <f>RIGHT(B19,LEN(B19)-1)</f>
+        <f t="shared" si="1"/>
         <v>Sales</v>
       </c>
       <c r="F19" t="str">
-        <f>"Branch "&amp;LEFT(B19,1)</f>
+        <f t="shared" si="2"/>
         <v>Branch 3</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>SaraSalesBranch 3</v>
       </c>
       <c r="I19" t="str">
@@ -3610,7 +3622,7 @@
         <v>HR</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>DavidHR</v>
       </c>
       <c r="N19">
@@ -3622,19 +3634,19 @@
       <c r="B20" t="str">
         <v>3HR</v>
       </c>
-      <c r="D20" s="23" t="str">
+      <c r="D20" s="17" t="str">
         <v>Stephen</v>
       </c>
       <c r="E20" t="str">
-        <f>RIGHT(B20,LEN(B20)-1)</f>
+        <f t="shared" si="1"/>
         <v>HR</v>
       </c>
       <c r="F20" t="str">
-        <f>"Branch "&amp;LEFT(B20,1)</f>
+        <f t="shared" si="2"/>
         <v>Branch 3</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>StephenHRBranch 3</v>
       </c>
     </row>
@@ -3643,19 +3655,19 @@
       <c r="B21" t="str">
         <v>3Finance</v>
       </c>
-      <c r="D21" s="23" t="str">
+      <c r="D21" s="17" t="str">
         <v>Mike</v>
       </c>
       <c r="E21" t="str">
-        <f>RIGHT(B21,LEN(B21)-1)</f>
+        <f t="shared" si="1"/>
         <v>Finance</v>
       </c>
       <c r="F21" t="str">
-        <f>"Branch "&amp;LEFT(B21,1)</f>
+        <f t="shared" si="2"/>
         <v>Branch 3</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>MikeFinanceBranch 3</v>
       </c>
     </row>
@@ -3664,19 +3676,19 @@
       <c r="B22" t="str">
         <v>4Sales</v>
       </c>
-      <c r="D22" s="23" t="str">
+      <c r="D22" s="17" t="str">
         <v>Sara</v>
       </c>
       <c r="E22" t="str">
-        <f>RIGHT(B22,LEN(B22)-1)</f>
+        <f t="shared" si="1"/>
         <v>Sales</v>
       </c>
       <c r="F22" t="str">
-        <f>"Branch "&amp;LEFT(B22,1)</f>
+        <f t="shared" si="2"/>
         <v>Branch 4</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>SaraSalesBranch 4</v>
       </c>
       <c r="M22" s="12" t="s">
@@ -3688,19 +3700,19 @@
       <c r="B23" s="16" t="str">
         <v>4HR</v>
       </c>
-      <c r="D23" s="24" t="str">
+      <c r="D23" s="18" t="str">
         <v>David</v>
       </c>
       <c r="E23" t="str">
-        <f>RIGHT(B23,LEN(B23)-1)</f>
+        <f t="shared" si="1"/>
         <v>HR</v>
       </c>
       <c r="F23" t="str">
-        <f>"Branch "&amp;LEFT(B23,1)</f>
+        <f t="shared" si="2"/>
         <v>Branch 4</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>DavidHRBranch 4</v>
       </c>
     </row>
@@ -3709,19 +3721,19 @@
       <c r="B24" s="16" t="str">
         <v>4Finance</v>
       </c>
-      <c r="D24" s="24" t="str">
+      <c r="D24" s="18" t="str">
         <v>Omid</v>
       </c>
       <c r="E24" t="str">
-        <f>RIGHT(B24,LEN(B24)-1)</f>
+        <f t="shared" si="1"/>
         <v>Finance</v>
       </c>
       <c r="F24" t="str">
-        <f>"Branch "&amp;LEFT(B24,1)</f>
+        <f t="shared" si="2"/>
         <v>Branch 4</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>OmidFinanceBranch 4</v>
       </c>
     </row>
@@ -4913,21 +4925,21 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="22"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="27"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1" t="s">
@@ -5319,7 +5331,7 @@
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="20" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="6"/>
@@ -6791,7 +6803,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6809,21 +6821,21 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="22"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="27"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1" t="s">
@@ -8437,8 +8449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18DBDBB5-2E9A-41A4-9F03-81DE029D39FA}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8449,28 +8461,28 @@
     <col min="5" max="5" width="12.09765625" customWidth="1"/>
     <col min="6" max="6" width="13.8984375" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" customWidth="1"/>
-    <col min="9" max="12" width="8" customWidth="1"/>
+    <col min="8" max="11" width="9.796875" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
     <col min="13" max="26" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="22"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="27"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1" t="s">
@@ -8776,7 +8788,7 @@
       <c r="A9" s="2"/>
       <c r="F9" s="6"/>
       <c r="G9" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>5</v>
@@ -8877,19 +8889,19 @@
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="27" t="s">
+      <c r="H15" s="21" t="s">
         <v>23</v>
       </c>
       <c r="N15">
@@ -8914,10 +8926,10 @@
       <c r="D16" t="str">
         <v>David</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="21" t="s">
         <v>24</v>
       </c>
       <c r="H16" t="s">
@@ -8959,14 +8971,13 @@
       <c r="G17" t="s">
         <v>3</v>
       </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28">
+      <c r="I17">
         <v>1</v>
       </c>
-      <c r="J17" s="28">
+      <c r="J17">
         <v>1</v>
       </c>
-      <c r="K17" s="28">
+      <c r="K17">
         <v>1</v>
       </c>
       <c r="N17">
@@ -8996,14 +9007,12 @@
       <c r="G18" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="28">
+      <c r="H18">
         <v>1</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18">
         <v>1</v>
       </c>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
       <c r="N18">
         <v>1</v>
       </c>
@@ -9031,12 +9040,9 @@
       <c r="G19" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28">
+      <c r="J19">
         <v>1</v>
       </c>
-      <c r="K19" s="28"/>
       <c r="N19">
         <v>2</v>
       </c>
@@ -9064,10 +9070,7 @@
       <c r="G20" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28">
+      <c r="K20">
         <v>1</v>
       </c>
       <c r="N20">
@@ -9097,12 +9100,9 @@
       <c r="G21" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="28">
+      <c r="H21">
         <v>1</v>
       </c>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
       <c r="N21">
         <v>1</v>
       </c>
@@ -9130,12 +9130,10 @@
       <c r="G22" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="28">
+      <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28">
+      <c r="K22">
         <v>1</v>
       </c>
       <c r="N22">
@@ -9166,14 +9164,12 @@
       <c r="G23" t="s">
         <v>5</v>
       </c>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28">
+      <c r="I23">
         <v>1</v>
       </c>
-      <c r="J23" s="28">
+      <c r="J23">
         <v>1</v>
       </c>
-      <c r="K23" s="28"/>
       <c r="N23">
         <v>3</v>
       </c>
@@ -9260,46 +9256,194 @@
       <c r="D27" t="str">
         <v>Omid</v>
       </c>
+      <c r="F27" s="7" t="str" cm="1">
+        <f t="array" ref="F27:K27">F16:K16</f>
+        <v>Name</v>
+      </c>
+      <c r="G27" s="7" t="str">
+        <v>Dept</v>
+      </c>
+      <c r="H27" s="28" t="str">
+        <v>1</v>
+      </c>
+      <c r="I27" s="28" t="str">
+        <v>2</v>
+      </c>
+      <c r="J27" s="28" t="str">
+        <v>3</v>
+      </c>
+      <c r="K27" s="28" t="str">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
+      <c r="F28" s="12" t="str" cm="1">
+        <f t="array" ref="F28:K34">INDEX(F17:K23,MATCH(G3:G9&amp;H3:H9,F17:F23&amp;G17:G23,0),{1,2,3,4,5,6})</f>
+        <v>David</v>
+      </c>
+      <c r="G28" s="12" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="H28" s="29">
+        <v>1</v>
+      </c>
+      <c r="I28" s="29">
+        <v>0</v>
+      </c>
+      <c r="J28" s="29">
+        <v>0</v>
+      </c>
+      <c r="K28" s="29">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
+      <c r="F29" s="12" t="str">
+        <v>Sara</v>
+      </c>
+      <c r="G29" s="12" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="H29" s="29">
+        <v>0</v>
+      </c>
+      <c r="I29" s="29">
+        <v>1</v>
+      </c>
+      <c r="J29" s="29">
+        <v>1</v>
+      </c>
+      <c r="K29" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
+      <c r="F30" s="12" t="str">
+        <v>Rose</v>
+      </c>
+      <c r="G30" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="H30" s="29">
+        <v>1</v>
+      </c>
+      <c r="I30" s="29">
+        <v>1</v>
+      </c>
+      <c r="J30" s="29">
+        <v>0</v>
+      </c>
+      <c r="K30" s="29">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
-    </row>
-    <row r="32" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="12" t="str">
+        <v>Stephen</v>
+      </c>
+      <c r="G31" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="H31" s="29">
+        <v>0</v>
+      </c>
+      <c r="I31" s="29">
+        <v>0</v>
+      </c>
+      <c r="J31" s="29">
+        <v>1</v>
+      </c>
+      <c r="K31" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="12" t="str">
+        <v>David</v>
+      </c>
+      <c r="G32" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="H32" s="29">
+        <v>0</v>
+      </c>
+      <c r="I32" s="29">
+        <v>0</v>
+      </c>
+      <c r="J32" s="29">
+        <v>0</v>
+      </c>
+      <c r="K32" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
-    </row>
-    <row r="34" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="12" t="str">
+        <v>Omid</v>
+      </c>
+      <c r="G33" s="12" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="H33" s="29">
+        <v>1</v>
+      </c>
+      <c r="I33" s="29">
+        <v>0</v>
+      </c>
+      <c r="J33" s="29">
+        <v>0</v>
+      </c>
+      <c r="K33" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F34" s="12" t="str">
+        <v>Mike</v>
+      </c>
+      <c r="G34" s="12" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="H34" s="29">
+        <v>0</v>
+      </c>
+      <c r="I34" s="29">
+        <v>1</v>
+      </c>
+      <c r="J34" s="29">
+        <v>1</v>
+      </c>
+      <c r="K34" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
     </row>
-    <row r="36" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
     </row>
-    <row r="37" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
     </row>
-    <row r="38" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
     </row>
-    <row r="39" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10258,6 +10402,6 @@
     <mergeCell ref="G1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More work with pivot functions
</commit_message>
<xml_diff>
--- a/CH-091 Extract from table.xlsx
+++ b/CH-091 Extract from table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0454BE75-D0A7-47FB-BFB4-27A268D183D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91BD7FF-8DA9-4CF8-A306-9431545BA523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
     <sheet name="Alt2" sheetId="6" r:id="rId4"/>
     <sheet name="PivotApproach" sheetId="7" r:id="rId5"/>
+    <sheet name="PivotFunctionApproach" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId6"/>
+    <pivotCache cacheId="15" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +40,7 @@
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="/I7b3y6w9dWI5DEUXeppQV2jUuCxrv3A0fktCS/dr1s="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="/I7b3y6w9dWI5DEUXeppQV2jUuCxrv3A0fktCS/dr1s="/>
     </ext>
   </extLst>
 </workbook>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="31">
   <si>
     <t>Question Table: Info</t>
   </si>
@@ -159,14 +160,17 @@
   <si>
     <t>Count of Branch</t>
   </si>
+  <si>
+    <t>Can I perform a custom sort on a pivot table?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="&quot;Branch &quot;@"/>
-    <numFmt numFmtId="167" formatCode="[=0]&quot;&quot;;[=1]\✔;"/>
+    <numFmt numFmtId="164" formatCode="&quot;Branch &quot;@"/>
+    <numFmt numFmtId="165" formatCode="[=0]&quot;&quot;;[=1]\✔;"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -543,6 +547,12 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -553,12 +563,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Intro_Hd" xfId="2" xr:uid="{DFD9014A-B813-42DF-BC0C-06DFCF29FB9F}"/>
@@ -1094,7 +1098,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{655F10CD-CF8F-48FE-8932-F26A00D2FD8F}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{655F10CD-CF8F-48FE-8932-F26A00D2FD8F}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="F15:K23" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -1443,21 +1447,21 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="27"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1" t="s">
@@ -2939,23 +2943,23 @@
   <sheetData>
     <row r="1" spans="1:28" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="27"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="29"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -4906,8 +4910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3E0D9B-0847-42B9-9F5A-45D930298918}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30:K41"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4925,21 +4929,21 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="27"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1" t="s">
@@ -6802,8 +6806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87663A00-0F87-4B43-9144-B85EE29B6E21}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6821,21 +6825,21 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="27"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1" t="s">
@@ -8449,8 +8453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18DBDBB5-2E9A-41A4-9F03-81DE029D39FA}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8468,21 +8472,21 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="27"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1" t="s">
@@ -9263,16 +9267,16 @@
       <c r="G27" s="7" t="str">
         <v>Dept</v>
       </c>
-      <c r="H27" s="28" t="str">
+      <c r="H27" s="22" t="str">
         <v>1</v>
       </c>
-      <c r="I27" s="28" t="str">
+      <c r="I27" s="22" t="str">
         <v>2</v>
       </c>
-      <c r="J27" s="28" t="str">
+      <c r="J27" s="22" t="str">
         <v>3</v>
       </c>
-      <c r="K27" s="28" t="str">
+      <c r="K27" s="22" t="str">
         <v>4</v>
       </c>
     </row>
@@ -9285,16 +9289,16 @@
       <c r="G28" s="12" t="str">
         <v>Sales</v>
       </c>
-      <c r="H28" s="29">
+      <c r="H28" s="23">
         <v>1</v>
       </c>
-      <c r="I28" s="29">
+      <c r="I28" s="23">
         <v>0</v>
       </c>
-      <c r="J28" s="29">
+      <c r="J28" s="23">
         <v>0</v>
       </c>
-      <c r="K28" s="29">
+      <c r="K28" s="23">
         <v>0</v>
       </c>
     </row>
@@ -9306,16 +9310,16 @@
       <c r="G29" s="12" t="str">
         <v>Sales</v>
       </c>
-      <c r="H29" s="29">
+      <c r="H29" s="23">
         <v>0</v>
       </c>
-      <c r="I29" s="29">
+      <c r="I29" s="23">
         <v>1</v>
       </c>
-      <c r="J29" s="29">
+      <c r="J29" s="23">
         <v>1</v>
       </c>
-      <c r="K29" s="29">
+      <c r="K29" s="23">
         <v>1</v>
       </c>
     </row>
@@ -9327,16 +9331,16 @@
       <c r="G30" s="12" t="str">
         <v>HR</v>
       </c>
-      <c r="H30" s="29">
+      <c r="H30" s="23">
         <v>1</v>
       </c>
-      <c r="I30" s="29">
+      <c r="I30" s="23">
         <v>1</v>
       </c>
-      <c r="J30" s="29">
+      <c r="J30" s="23">
         <v>0</v>
       </c>
-      <c r="K30" s="29">
+      <c r="K30" s="23">
         <v>0</v>
       </c>
     </row>
@@ -9348,16 +9352,16 @@
       <c r="G31" s="12" t="str">
         <v>HR</v>
       </c>
-      <c r="H31" s="29">
+      <c r="H31" s="23">
         <v>0</v>
       </c>
-      <c r="I31" s="29">
+      <c r="I31" s="23">
         <v>0</v>
       </c>
-      <c r="J31" s="29">
+      <c r="J31" s="23">
         <v>1</v>
       </c>
-      <c r="K31" s="29">
+      <c r="K31" s="23">
         <v>0</v>
       </c>
     </row>
@@ -9368,16 +9372,16 @@
       <c r="G32" s="12" t="str">
         <v>HR</v>
       </c>
-      <c r="H32" s="29">
+      <c r="H32" s="23">
         <v>0</v>
       </c>
-      <c r="I32" s="29">
+      <c r="I32" s="23">
         <v>0</v>
       </c>
-      <c r="J32" s="29">
+      <c r="J32" s="23">
         <v>0</v>
       </c>
-      <c r="K32" s="29">
+      <c r="K32" s="23">
         <v>1</v>
       </c>
     </row>
@@ -9389,16 +9393,16 @@
       <c r="G33" s="12" t="str">
         <v>Finance</v>
       </c>
-      <c r="H33" s="29">
+      <c r="H33" s="23">
         <v>1</v>
       </c>
-      <c r="I33" s="29">
+      <c r="I33" s="23">
         <v>0</v>
       </c>
-      <c r="J33" s="29">
+      <c r="J33" s="23">
         <v>0</v>
       </c>
-      <c r="K33" s="29">
+      <c r="K33" s="23">
         <v>1</v>
       </c>
     </row>
@@ -9409,16 +9413,16 @@
       <c r="G34" s="12" t="str">
         <v>Finance</v>
       </c>
-      <c r="H34" s="29">
+      <c r="H34" s="23">
         <v>0</v>
       </c>
-      <c r="I34" s="29">
+      <c r="I34" s="23">
         <v>1</v>
       </c>
-      <c r="J34" s="29">
+      <c r="J34" s="23">
         <v>1</v>
       </c>
-      <c r="K34" s="29">
+      <c r="K34" s="23">
         <v>0</v>
       </c>
     </row>
@@ -10404,4 +10408,1901 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44F8F24-9131-4266-952F-8C341B649CE5}">
+  <dimension ref="A1:Z1000"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="4" width="12.3984375" customWidth="1"/>
+    <col min="5" max="5" width="12.09765625" customWidth="1"/>
+    <col min="6" max="6" width="13.8984375" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="11.3984375" customWidth="1"/>
+    <col min="9" max="12" width="9.69921875" customWidth="1"/>
+    <col min="13" max="26" width="8.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+    </row>
+    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+    </row>
+    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="13">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+    </row>
+    <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="13">
+        <v>3</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+    </row>
+    <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="13">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+    </row>
+    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+    </row>
+    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+    </row>
+    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="12"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+    </row>
+    <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+    </row>
+    <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+    </row>
+    <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="S12" s="6"/>
+    </row>
+    <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="S13" s="6"/>
+    </row>
+    <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="7" t="str" cm="1">
+        <f t="array" ref="G15:L22">_xlfn.DROP(_xlfn.DROP(_xlfn.PIVOTBY(D16:E27,C16:C27,C16:C27,_xleta.COUNTA),-1),,-1)</f>
+        <v/>
+      </c>
+      <c r="H15" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I15" s="22" t="str">
+        <v>1</v>
+      </c>
+      <c r="J15" s="22" t="str">
+        <v>2</v>
+      </c>
+      <c r="K15" s="22" t="str">
+        <v>3</v>
+      </c>
+      <c r="L15" s="22" t="str">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="12" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="H16" s="12" t="str">
+        <v>Mike</v>
+      </c>
+      <c r="I16" s="23" t="str">
+        <v/>
+      </c>
+      <c r="J16" s="23">
+        <v>1</v>
+      </c>
+      <c r="K16" s="23">
+        <v>1</v>
+      </c>
+      <c r="L16" s="23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="12" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="H17" s="12" t="str">
+        <v>Omid</v>
+      </c>
+      <c r="I17" s="23">
+        <v>1</v>
+      </c>
+      <c r="J17" s="23" t="str">
+        <v/>
+      </c>
+      <c r="K17" s="23" t="str">
+        <v/>
+      </c>
+      <c r="L17" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="H18" s="12" t="str">
+        <v>David</v>
+      </c>
+      <c r="I18" s="23" t="str">
+        <v/>
+      </c>
+      <c r="J18" s="23" t="str">
+        <v/>
+      </c>
+      <c r="K18" s="23" t="str">
+        <v/>
+      </c>
+      <c r="L18" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="H19" s="12" t="str">
+        <v>Rose</v>
+      </c>
+      <c r="I19" s="23">
+        <v>1</v>
+      </c>
+      <c r="J19" s="23">
+        <v>1</v>
+      </c>
+      <c r="K19" s="23" t="str">
+        <v/>
+      </c>
+      <c r="L19" s="23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="H20" s="12" t="str">
+        <v>Stephen</v>
+      </c>
+      <c r="I20" s="23" t="str">
+        <v/>
+      </c>
+      <c r="J20" s="23" t="str">
+        <v/>
+      </c>
+      <c r="K20" s="23">
+        <v>1</v>
+      </c>
+      <c r="L20" s="23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="12" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="H21" s="12" t="str">
+        <v>David</v>
+      </c>
+      <c r="I21" s="23">
+        <v>1</v>
+      </c>
+      <c r="J21" s="23" t="str">
+        <v/>
+      </c>
+      <c r="K21" s="23" t="str">
+        <v/>
+      </c>
+      <c r="L21" s="23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="12" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="H22" s="12" t="str">
+        <v>Sara</v>
+      </c>
+      <c r="I22" s="23" t="str">
+        <v/>
+      </c>
+      <c r="J22" s="23">
+        <v>1</v>
+      </c>
+      <c r="K22" s="23">
+        <v>1</v>
+      </c>
+      <c r="L22" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="7" t="str" cm="1">
+        <f t="array" ref="G27:L34">_xlfn.VSTACK({"Dept","Name","1","2","3","4"},INDEX(G16:L22,_xlfn.XMATCH(G3:G9&amp;H3:H9,H16:H22&amp;G16:G22,0),{2,1,3,4,5,6}))</f>
+        <v>Dept</v>
+      </c>
+      <c r="H27" s="7" t="str">
+        <v>Name</v>
+      </c>
+      <c r="I27" s="22" t="str">
+        <v>1</v>
+      </c>
+      <c r="J27" s="22" t="str">
+        <v>2</v>
+      </c>
+      <c r="K27" s="22" t="str">
+        <v>3</v>
+      </c>
+      <c r="L27" s="22" t="str">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
+      <c r="G28" s="12" t="str">
+        <v>David</v>
+      </c>
+      <c r="H28" s="12" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="I28" s="23">
+        <v>1</v>
+      </c>
+      <c r="J28" s="23" t="str">
+        <v/>
+      </c>
+      <c r="K28" s="23" t="str">
+        <v/>
+      </c>
+      <c r="L28" s="23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+      <c r="G29" s="12" t="str">
+        <v>Sara</v>
+      </c>
+      <c r="H29" s="12" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="I29" s="23" t="str">
+        <v/>
+      </c>
+      <c r="J29" s="23">
+        <v>1</v>
+      </c>
+      <c r="K29" s="23">
+        <v>1</v>
+      </c>
+      <c r="L29" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="G30" s="12" t="str">
+        <v>Rose</v>
+      </c>
+      <c r="H30" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="I30" s="23">
+        <v>1</v>
+      </c>
+      <c r="J30" s="23">
+        <v>1</v>
+      </c>
+      <c r="K30" s="23" t="str">
+        <v/>
+      </c>
+      <c r="L30" s="23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="G31" s="12" t="str">
+        <v>Stephen</v>
+      </c>
+      <c r="H31" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="I31" s="23" t="str">
+        <v/>
+      </c>
+      <c r="J31" s="23" t="str">
+        <v/>
+      </c>
+      <c r="K31" s="23">
+        <v>1</v>
+      </c>
+      <c r="L31" s="23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="12" t="str">
+        <v>David</v>
+      </c>
+      <c r="H32" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="I32" s="23" t="str">
+        <v/>
+      </c>
+      <c r="J32" s="23" t="str">
+        <v/>
+      </c>
+      <c r="K32" s="23" t="str">
+        <v/>
+      </c>
+      <c r="L32" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+      <c r="G33" s="12" t="str">
+        <v>Omid</v>
+      </c>
+      <c r="H33" s="12" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="I33" s="23">
+        <v>1</v>
+      </c>
+      <c r="J33" s="23" t="str">
+        <v/>
+      </c>
+      <c r="K33" s="23" t="str">
+        <v/>
+      </c>
+      <c r="L33" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="12" t="str">
+        <v>Mike</v>
+      </c>
+      <c r="H34" s="12" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="I34" s="23" t="str">
+        <v/>
+      </c>
+      <c r="J34" s="23">
+        <v>1</v>
+      </c>
+      <c r="K34" s="23">
+        <v>1</v>
+      </c>
+      <c r="L34" s="23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+    </row>
+    <row r="36" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+    </row>
+    <row r="37" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+    </row>
+    <row r="38" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+    </row>
+    <row r="39" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
I used a custom function in the pivot table
</commit_message>
<xml_diff>
--- a/CH-091 Extract from table.xlsx
+++ b/CH-091 Extract from table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91BD7FF-8DA9-4CF8-A306-9431545BA523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDFA868-051B-4273-B55C-B5F7062DEBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="Alt2" sheetId="6" r:id="rId4"/>
     <sheet name="PivotApproach" sheetId="7" r:id="rId5"/>
     <sheet name="PivotFunctionApproach" sheetId="8" r:id="rId6"/>
+    <sheet name="PivotFunctionApproach2" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId7"/>
+    <pivotCache cacheId="16" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +41,7 @@
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="/I7b3y6w9dWI5DEUXeppQV2jUuCxrv3A0fktCS/dr1s="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="/I7b3y6w9dWI5DEUXeppQV2jUuCxrv3A0fktCS/dr1s="/>
     </ext>
   </extLst>
 </workbook>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="31">
   <si>
     <t>Question Table: Info</t>
   </si>
@@ -1098,7 +1099,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{655F10CD-CF8F-48FE-8932-F26A00D2FD8F}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{655F10CD-CF8F-48FE-8932-F26A00D2FD8F}" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="F15:K23" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -10414,8 +10415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44F8F24-9131-4266-952F-8C341B649CE5}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11318,6 +11319,1903 @@
       </c>
       <c r="K34" s="23">
         <v>1</v>
+      </c>
+      <c r="L34" s="23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+    </row>
+    <row r="36" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+    </row>
+    <row r="37" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+    </row>
+    <row r="38" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+    </row>
+    <row r="39" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490E5256-16C9-4345-A6E7-AFA30D2B3A77}">
+  <dimension ref="A1:Z1000"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="4" width="12.3984375" customWidth="1"/>
+    <col min="5" max="5" width="12.09765625" customWidth="1"/>
+    <col min="6" max="6" width="13.8984375" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="11.3984375" customWidth="1"/>
+    <col min="9" max="12" width="9.69921875" customWidth="1"/>
+    <col min="13" max="26" width="8.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+    </row>
+    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+    </row>
+    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="13">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+    </row>
+    <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="13">
+        <v>3</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+    </row>
+    <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="13">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+    </row>
+    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+    </row>
+    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+    </row>
+    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="12"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+    </row>
+    <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+    </row>
+    <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+    </row>
+    <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="S12" s="6"/>
+    </row>
+    <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="S13" s="6"/>
+    </row>
+    <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="7" t="str" cm="1">
+        <f t="array" ref="G15:L22">_xlfn.DROP(_xlfn.DROP(_xlfn.PIVOTBY(D16:E27,C16:C27,C16:C27,_xlfn.LAMBDA(_xlpm.x,IF(COUNTA(_xlpm.x),"✔",""))),-1),,-1)</f>
+        <v/>
+      </c>
+      <c r="H15" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I15" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="J15" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="K15" s="7" t="str">
+        <v>3</v>
+      </c>
+      <c r="L15" s="7" t="str">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="12" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="H16" s="12" t="str">
+        <v>Mike</v>
+      </c>
+      <c r="I16" s="12" t="str">
+        <v/>
+      </c>
+      <c r="J16" s="12" t="str">
+        <v>✔</v>
+      </c>
+      <c r="K16" s="12" t="str">
+        <v>✔</v>
+      </c>
+      <c r="L16" s="12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="12" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="H17" s="12" t="str">
+        <v>Omid</v>
+      </c>
+      <c r="I17" s="12" t="str">
+        <v>✔</v>
+      </c>
+      <c r="J17" s="12" t="str">
+        <v/>
+      </c>
+      <c r="K17" s="12" t="str">
+        <v/>
+      </c>
+      <c r="L17" s="12" t="str">
+        <v>✔</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="H18" s="12" t="str">
+        <v>David</v>
+      </c>
+      <c r="I18" s="12" t="str">
+        <v/>
+      </c>
+      <c r="J18" s="12" t="str">
+        <v/>
+      </c>
+      <c r="K18" s="12" t="str">
+        <v/>
+      </c>
+      <c r="L18" s="12" t="str">
+        <v>✔</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="H19" s="12" t="str">
+        <v>Rose</v>
+      </c>
+      <c r="I19" s="12" t="str">
+        <v>✔</v>
+      </c>
+      <c r="J19" s="12" t="str">
+        <v>✔</v>
+      </c>
+      <c r="K19" s="12" t="str">
+        <v/>
+      </c>
+      <c r="L19" s="12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="H20" s="12" t="str">
+        <v>Stephen</v>
+      </c>
+      <c r="I20" s="12" t="str">
+        <v/>
+      </c>
+      <c r="J20" s="12" t="str">
+        <v/>
+      </c>
+      <c r="K20" s="12" t="str">
+        <v>✔</v>
+      </c>
+      <c r="L20" s="12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="12" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="H21" s="12" t="str">
+        <v>David</v>
+      </c>
+      <c r="I21" s="12" t="str">
+        <v>✔</v>
+      </c>
+      <c r="J21" s="12" t="str">
+        <v/>
+      </c>
+      <c r="K21" s="12" t="str">
+        <v/>
+      </c>
+      <c r="L21" s="12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="12" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="H22" s="12" t="str">
+        <v>Sara</v>
+      </c>
+      <c r="I22" s="12" t="str">
+        <v/>
+      </c>
+      <c r="J22" s="12" t="str">
+        <v>✔</v>
+      </c>
+      <c r="K22" s="12" t="str">
+        <v>✔</v>
+      </c>
+      <c r="L22" s="12" t="str">
+        <v>✔</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="7" t="str" cm="1">
+        <f t="array" ref="G27:L34">_xlfn.VSTACK({"Dept","Name","1","2","3","4"},INDEX(G16:L22,_xlfn.XMATCH(G3:G9&amp;H3:H9,H16:H22&amp;G16:G22,0),{2,1,3,4,5,6}))</f>
+        <v>Dept</v>
+      </c>
+      <c r="H27" s="7" t="str">
+        <v>Name</v>
+      </c>
+      <c r="I27" s="22" t="str">
+        <v>1</v>
+      </c>
+      <c r="J27" s="22" t="str">
+        <v>2</v>
+      </c>
+      <c r="K27" s="22" t="str">
+        <v>3</v>
+      </c>
+      <c r="L27" s="22" t="str">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
+      <c r="G28" s="12" t="str">
+        <v>David</v>
+      </c>
+      <c r="H28" s="12" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="I28" s="23" t="str">
+        <v>✔</v>
+      </c>
+      <c r="J28" s="23" t="str">
+        <v/>
+      </c>
+      <c r="K28" s="23" t="str">
+        <v/>
+      </c>
+      <c r="L28" s="23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+      <c r="G29" s="12" t="str">
+        <v>Sara</v>
+      </c>
+      <c r="H29" s="12" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="I29" s="23" t="str">
+        <v/>
+      </c>
+      <c r="J29" s="23" t="str">
+        <v>✔</v>
+      </c>
+      <c r="K29" s="23" t="str">
+        <v>✔</v>
+      </c>
+      <c r="L29" s="23" t="str">
+        <v>✔</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="G30" s="12" t="str">
+        <v>Rose</v>
+      </c>
+      <c r="H30" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="I30" s="23" t="str">
+        <v>✔</v>
+      </c>
+      <c r="J30" s="23" t="str">
+        <v>✔</v>
+      </c>
+      <c r="K30" s="23" t="str">
+        <v/>
+      </c>
+      <c r="L30" s="23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="G31" s="12" t="str">
+        <v>Stephen</v>
+      </c>
+      <c r="H31" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="I31" s="23" t="str">
+        <v/>
+      </c>
+      <c r="J31" s="23" t="str">
+        <v/>
+      </c>
+      <c r="K31" s="23" t="str">
+        <v>✔</v>
+      </c>
+      <c r="L31" s="23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="12" t="str">
+        <v>David</v>
+      </c>
+      <c r="H32" s="12" t="str">
+        <v>HR</v>
+      </c>
+      <c r="I32" s="23" t="str">
+        <v/>
+      </c>
+      <c r="J32" s="23" t="str">
+        <v/>
+      </c>
+      <c r="K32" s="23" t="str">
+        <v/>
+      </c>
+      <c r="L32" s="23" t="str">
+        <v>✔</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+      <c r="G33" s="12" t="str">
+        <v>Omid</v>
+      </c>
+      <c r="H33" s="12" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="I33" s="23" t="str">
+        <v>✔</v>
+      </c>
+      <c r="J33" s="23" t="str">
+        <v/>
+      </c>
+      <c r="K33" s="23" t="str">
+        <v/>
+      </c>
+      <c r="L33" s="23" t="str">
+        <v>✔</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="12" t="str">
+        <v>Mike</v>
+      </c>
+      <c r="H34" s="12" t="str">
+        <v>Finance</v>
+      </c>
+      <c r="I34" s="23" t="str">
+        <v/>
+      </c>
+      <c r="J34" s="23" t="str">
+        <v>✔</v>
+      </c>
+      <c r="K34" s="23" t="str">
+        <v>✔</v>
       </c>
       <c r="L34" s="23" t="str">
         <v/>

</xml_diff>